<commit_message>
changed from_tree to take names of lambda. lambda now a series
</commit_message>
<xml_diff>
--- a/data/input/tree/meaningfulness/weights_0.xlsx
+++ b/data/input/tree/meaningfulness/weights_0.xlsx
@@ -22,13 +22,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
   <si>
-    <t xml:space="preserve">ecological_parameters</t>
+    <t xml:space="preserve">ecology</t>
   </si>
   <si>
-    <t xml:space="preserve">mechanical_parameters</t>
+    <t xml:space="preserve">mechanical</t>
   </si>
   <si>
-    <t xml:space="preserve">process_parameters</t>
+    <t xml:space="preserve">process</t>
   </si>
 </sst>
 </file>
@@ -139,15 +139,15 @@
   <dimension ref="A1:D1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="10.5"/>
   </cols>
   <sheetData>

</xml_diff>